<commit_message>
Begin on skill performing
</commit_message>
<xml_diff>
--- a/Assets/Game/Skills.xlsx
+++ b/Assets/Game/Skills.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Otter\Assets\Game\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A80D59-7B57-4D61-8061-1968398446EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2256EEA0-C484-4210-A552-889731F66797}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5130" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1349,8 +1349,8 @@
   <dimension ref="A1:L140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I76" sqref="I76"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>